<commit_message>
Add additional table to spreadsheet
</commit_message>
<xml_diff>
--- a/ct4.xlsx
+++ b/ct4.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcoe02/src/pcr/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AAE135E3-4259-A743-B064-15F3DEA1B789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BE2361-0414-2B4D-B8D7-6254256652B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{AD557002-837B-F545-878B-34144364B9F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="10">
   <si>
     <t>Sample</t>
   </si>
@@ -55,6 +56,15 @@
   </si>
   <si>
     <t>Concentration</t>
+  </si>
+  <si>
+    <t>Ct</t>
+  </si>
+  <si>
+    <t>Gene</t>
+  </si>
+  <si>
+    <t>Replicate</t>
   </si>
 </sst>
 </file>
@@ -118,6 +128,20 @@
     <tableColumn id="3" xr3:uid="{7118956C-A27C-3E47-916B-CECF5CB74700}" name="Concentration"/>
     <tableColumn id="4" xr3:uid="{E18DB224-D864-8A4E-9A7E-057073B54B2E}" name="Target"/>
     <tableColumn id="5" xr3:uid="{52D8211B-10C1-FE48-B7FF-71772927895B}" name="Reference"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6F068C70-6F00-9E44-A05F-21C497B8E571}" name="Table1" displayName="Table1" ref="A1:E49" totalsRowShown="0">
+  <autoFilter ref="A1:E49" xr:uid="{6F068C70-6F00-9E44-A05F-21C497B8E571}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{270862D5-7DDD-8041-A477-A039AE4BEF5A}" name="Group"/>
+    <tableColumn id="2" xr3:uid="{D66DBF97-DFC7-0947-8A1A-85171016AAE7}" name="Gene"/>
+    <tableColumn id="3" xr3:uid="{56B0C13D-597A-654F-9B05-D61043429FBB}" name="Concentration"/>
+    <tableColumn id="5" xr3:uid="{5F9D5835-B2EC-F24B-B3DF-7DC3BBEBD8A4}" name="Replicate"/>
+    <tableColumn id="4" xr3:uid="{2488E680-5E08-B842-8AA0-FF5F0664F8F2}" name="Ct"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -423,7 +447,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -865,4 +889,856 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5366D9BA-FBB3-A44B-9239-8574A4FAF3D9}">
+  <dimension ref="A1:E49"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>23.110199999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>22.900300000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>22.897200000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>26.580100000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>26.213899999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>26.060600000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>0.4</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>28.112500000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>0.4</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>28.189900000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>0.4</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>27.594899999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>0.08</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>30.277200000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>0.08</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>30.466699999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>0.08</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>30.757100000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>21.781300000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>21.756399999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>21.640999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>23.796500000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18">
+        <v>23.757100000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>23.724</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>0.4</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>26.3794</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>0.4</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>26.254200000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>0.4</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>25.9621</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>0.08</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>28.547899999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>0.08</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>28.389399999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>0.08</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>28.3416</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>19.741499999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27">
+        <v>19.494</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>10</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <v>19.390599999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>21.983799999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <v>22.4435</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <v>22.57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>0.4</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>24.8109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>0.4</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33">
+        <v>24.432700000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <v>0.4</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34">
+        <v>24.234200000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>0.08</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>26.7319</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <v>0.08</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="E36">
+        <v>26.820599999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <v>0.08</v>
+      </c>
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <v>26.821999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>10</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>18.4468</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39">
+        <v>10</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>18.822700000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40">
+        <v>10</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="E40">
+        <v>18.306100000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>21.256799999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="E42">
+        <v>21.095600000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43">
+        <v>20.847300000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44">
+        <v>0.4</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>23.232199999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <v>0.4</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45">
+        <v>22.957699999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <v>0.4</v>
+      </c>
+      <c r="D46">
+        <v>3</v>
+      </c>
+      <c r="E46">
+        <v>23.241499999999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <v>0.08</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>25.4817</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" t="s">
+        <v>3</v>
+      </c>
+      <c r="C48">
+        <v>0.08</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <v>25.608000000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3</v>
+      </c>
+      <c r="C49">
+        <v>0.08</v>
+      </c>
+      <c r="D49">
+        <v>3</v>
+      </c>
+      <c r="E49">
+        <v>25.567499999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>